<commit_message>
Ultimo aggiornamento per il test 62
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111XXXX646502CIAFFI_SRL/CIAFFI_SRL/LUITECOLAB/2.2/report-checklist.xlsx
+++ b/GATEWAY/A1#111XXXX646502CIAFFI_SRL/CIAFFI_SRL/LUITECOLAB/2.2/report-checklist.xlsx
@@ -649,13 +649,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 16" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-06-19T17:47:06Z</t>
-  </si>
-  <si>
-    <t>d68336f017a5eaea72aea01d250a4931</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.36b752291d7ee2dc9561b9ac59cd51f261a178cbc78d7ab2c2415ef6cdeef302.f8d2a46dd8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-06-19T19:56:55Z</t>
+  </si>
+  <si>
+    <t>a8594cace05eb9fdef4c69f7edbbb5aa</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.25413009308a4bae125585955d301f246db200fe149e896215630000f3b5c431.9516b30c04^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>ATTENZIONE MANCA LA SPECIFICA DEL CODICE DELL'ESAME ISOLATO</t>
@@ -1851,10 +1851,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="d/m/yyyy"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="34">
     <font>
@@ -1935,50 +1935,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2000,9 +1972,54 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2016,23 +2033,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2047,14 +2049,6 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -2062,17 +2056,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2127,7 +2127,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2139,25 +2235,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2169,19 +2283,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2193,121 +2295,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2634,8 +2634,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2655,24 +2655,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -2684,6 +2666,17 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2703,6 +2696,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -2717,163 +2728,152 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="29" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="30" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="25" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="32" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -4511,7 +4511,7 @@
   <dimension ref="A1:W752"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="R10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="G10" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>

</xml_diff>